<commit_message>
Update README and dial notebooks: Enhance README.md with new dial generation and application instructions. Modify dial.ipynb to reset execution counts and update dial function calls. Revise quant_workflows_notebook.ipynb to reflect new configuration dates and commands for various deal types, including SSS and CRT processing commands.
</commit_message>
<xml_diff>
--- a/dial/outputs/dial_ratio_by_deal_6M_edit.xlsx
+++ b/dial/outputs/dial_ratio_by_deal_6M_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hzeng\Desktop\howard-toolbox\dial\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE3E4A7-FEAE-48FD-BF13-4D11712A15E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEA2999-65B9-45F2-9296-2C09ECD6B1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15345" yWindow="-150" windowWidth="44655" windowHeight="21285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4965" yWindow="-20595" windowWidth="49725" windowHeight="21285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STACR" sheetId="1" r:id="rId1"/>
@@ -672,9 +672,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R30" sqref="R30"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +884,7 @@
         <v>0.78783123830167434</v>
       </c>
       <c r="M5" s="5">
-        <v>0.8105837886765761</v>
+        <v>0.81058378867657599</v>
       </c>
       <c r="N5" s="5">
         <v>0.78783123830167434</v>
@@ -933,11 +933,11 @@
         <v>1.3151039891753009</v>
       </c>
       <c r="N6" s="9">
-        <v>1.3151039891753009</v>
+        <v>1.3151039891753</v>
       </c>
       <c r="O6" s="8">
         <f t="shared" si="0"/>
-        <v>-0.13806837222871704</v>
+        <v>-0.13806837222871793</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -979,11 +979,11 @@
         <v>0.68948767601745409</v>
       </c>
       <c r="N7" s="5">
-        <v>0.68948767601745409</v>
+        <v>0.68948767601745398</v>
       </c>
       <c r="O7" s="4">
         <f t="shared" si="0"/>
-        <v>0.10035644676503208</v>
+        <v>0.10035644676503197</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1025,11 +1025,11 @@
         <v>0.85454022157930476</v>
       </c>
       <c r="N8" s="9">
-        <v>0.90961034143516595</v>
+        <v>0.85454022157930498</v>
       </c>
       <c r="O8" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-5.5070119855860966E-2</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1209,11 +1209,11 @@
         <v>0.44183307923031739</v>
       </c>
       <c r="N12" s="9">
-        <v>0.44183307923031739</v>
+        <v>0.44183307923031701</v>
       </c>
       <c r="O12" s="8">
         <f t="shared" si="0"/>
-        <v>-0.17841554226918582</v>
+        <v>-0.17841554226918621</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1255,11 +1255,11 @@
         <v>1.0224798890822071</v>
       </c>
       <c r="N13" s="5">
-        <v>1.0224798890822071</v>
+        <v>1.02247988908221</v>
       </c>
       <c r="O13" s="4">
         <f t="shared" si="0"/>
-        <v>-8.0231689930026828E-2</v>
+        <v>-8.0231689930023942E-2</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1393,11 +1393,11 @@
         <v>0.91520352396647675</v>
       </c>
       <c r="N16" s="9">
-        <v>0.99739489748299182</v>
+        <v>0.91520352396647697</v>
       </c>
       <c r="O16" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-8.2191373516514843E-2</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1531,11 +1531,11 @@
         <v>1.7077763791853791</v>
       </c>
       <c r="N19" s="5">
-        <v>1.7077763791853791</v>
+        <v>1.7077763791853799</v>
       </c>
       <c r="O19" s="4">
         <f t="shared" si="0"/>
-        <v>0.35615078370356312</v>
+        <v>0.35615078370356401</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1577,11 +1577,11 @@
         <v>1.352718341503433</v>
       </c>
       <c r="N20" s="9">
-        <v>1.352718341503433</v>
+        <v>1.3527183415034301</v>
       </c>
       <c r="O20" s="8">
         <f t="shared" si="0"/>
-        <v>0.10953965558046597</v>
+        <v>0.10953965558046308</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1853,11 +1853,11 @@
         <v>1.487047447193091</v>
       </c>
       <c r="N26" s="9">
-        <v>1.487047447193091</v>
+        <v>1.4870474471930899</v>
       </c>
       <c r="O26" s="8">
         <f t="shared" si="0"/>
-        <v>0.13605878111760705</v>
+        <v>0.13605878111760594</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2129,11 +2129,11 @@
         <v>1.138682291755128</v>
       </c>
       <c r="N32" s="9">
-        <v>1.138682291755128</v>
+        <v>1.13868229175513</v>
       </c>
       <c r="O32" s="8">
         <f t="shared" si="0"/>
-        <v>0.13868929093000959</v>
+        <v>0.13868929093001159</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2175,11 +2175,11 @@
         <v>1.2109948087935949</v>
       </c>
       <c r="N33" s="5">
-        <v>1.2109948087935949</v>
+        <v>1.21099480879359</v>
       </c>
       <c r="O33" s="4">
         <f t="shared" si="0"/>
-        <v>0.21099480879359489</v>
+        <v>0.21099480879359001</v>
       </c>
     </row>
   </sheetData>
@@ -2231,9 +2231,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2584,11 +2584,11 @@
         <v>0.88759591484851674</v>
       </c>
       <c r="N8" s="9">
-        <v>0.88759591484851674</v>
+        <v>0.88759591484851696</v>
       </c>
       <c r="O8" s="8">
         <f t="shared" si="0"/>
-        <v>-9.2184409017092683E-2</v>
+        <v>-9.2184409017092461E-2</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2768,11 +2768,11 @@
         <v>0.39252693080556322</v>
       </c>
       <c r="N12" s="9">
-        <v>0.39252693080556322</v>
+        <v>0.392526930805563</v>
       </c>
       <c r="O12" s="8">
         <f t="shared" si="0"/>
-        <v>-0.2279489182896971</v>
+        <v>-0.22794891828969732</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2814,11 +2814,11 @@
         <v>0.89398782046780623</v>
       </c>
       <c r="N13" s="5">
-        <v>0.89398782046780623</v>
+        <v>0.893987820467806</v>
       </c>
       <c r="O13" s="4">
         <f t="shared" si="0"/>
-        <v>-8.5809093658035573E-2</v>
+        <v>-8.5809093658035795E-2</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2998,11 +2998,11 @@
         <v>1.0561866341376711</v>
       </c>
       <c r="N17" s="5">
-        <v>1.0561866341376711</v>
+        <v>1.05618663413767</v>
       </c>
       <c r="O17" s="4">
         <f t="shared" si="0"/>
-        <v>3.6246931001169047E-2</v>
+        <v>3.6246931001167937E-2</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -3274,11 +3274,11 @@
         <v>0.5226772929334651</v>
       </c>
       <c r="N23" s="5">
-        <v>0.60431452922472229</v>
+        <v>0.52267729293346499</v>
       </c>
       <c r="O23" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-8.1637236291257298E-2</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -3366,11 +3366,11 @@
         <v>1.320004151436504</v>
       </c>
       <c r="N25" s="5">
-        <v>1.320004151436504</v>
+        <v>1.3200041514365</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="0"/>
-        <v>-0.14646397947241008</v>
+        <v>-0.14646397947241407</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update README and dial scripts: Revise README.md to include new quick start instructions for the Dial Command Generator. Enhance dial.ipynb with a markdown cell for command generation and update execution counts. Modify update_dials.py to handle identity dials and improve version handling. Adjust quant_workflows_notebook.ipynb to reflect updated command structures and deal types.
</commit_message>
<xml_diff>
--- a/dial/outputs/dial_ratio_by_deal_6M_edit.xlsx
+++ b/dial/outputs/dial_ratio_by_deal_6M_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hzeng\Desktop\howard-toolbox\dial\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEA2999-65B9-45F2-9296-2C09ECD6B1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F57619-8639-4345-8FF5-53ADAB3FEA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4965" yWindow="-20595" windowWidth="49725" windowHeight="21285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-195" yWindow="-13125" windowWidth="44655" windowHeight="21285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STACR" sheetId="1" r:id="rId1"/>
@@ -674,7 +674,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4868,7 +4868,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:O20"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4992,11 +4992,11 @@
         <v>0.96398899888118861</v>
       </c>
       <c r="N3" s="5">
-        <v>0.96398899888118861</v>
+        <v>0.96398899888118905</v>
       </c>
       <c r="O3" s="4">
         <f t="shared" ref="O3:O20" si="0">N3-L3</f>
-        <v>0.10906315085985163</v>
+        <v>0.10906315085985208</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -5176,11 +5176,11 @@
         <v>0.87660034734774628</v>
       </c>
       <c r="N7" s="5">
-        <v>0.87660034734774628</v>
+        <v>0.87660034734774595</v>
       </c>
       <c r="O7" s="4">
         <f t="shared" si="0"/>
-        <v>-0.12252706367132027</v>
+        <v>-0.1225270636713206</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -5222,11 +5222,11 @@
         <v>0.67835769439909122</v>
       </c>
       <c r="N8" s="9">
-        <v>0.67835769439909122</v>
+        <v>0.67835769439909099</v>
       </c>
       <c r="O8" s="8">
         <f t="shared" si="0"/>
-        <v>-0.1496749469444596</v>
+        <v>-0.14967494694445982</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -5268,11 +5268,11 @@
         <v>0.66123592422645716</v>
       </c>
       <c r="N9" s="5">
-        <v>0.66123592422645716</v>
+        <v>0.66123592422645705</v>
       </c>
       <c r="O9" s="4">
         <f t="shared" si="0"/>
-        <v>-0.13928091965257428</v>
+        <v>-0.13928091965257439</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -5544,11 +5544,11 @@
         <v>0.68726931661501489</v>
       </c>
       <c r="N15" s="5">
-        <v>0.68726931661501489</v>
+        <v>0.687269316615015</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" si="0"/>
-        <v>0.43050228342449848</v>
+        <v>0.43050228342449859</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -5636,11 +5636,11 @@
         <v>0.61115427888447038</v>
       </c>
       <c r="N17" s="5">
-        <v>0.61115427888447038</v>
+        <v>0.61115427888447005</v>
       </c>
       <c r="O17" s="4">
         <f t="shared" si="0"/>
-        <v>0.101619736169274</v>
+        <v>0.10161973616927367</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -5832,7 +5832,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>